<commit_message>
Add scenario to repository
</commit_message>
<xml_diff>
--- a/project_open_entrance/00_base_model_setup/data/Eldata.xlsx
+++ b/project_open_entrance/00_base_model_setup/data/Eldata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beukeladvd\Documents\GitHub\tno-eco-mod-ci\project_open_entrance\00_base_model_setup\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boonmanhj\Documents\Gitlab\TNO-Eco-Mod-CI\project_open_entrance\00_base_model_setup\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D506A3-BC33-49A7-8EF9-0B472EEBA0C1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D6F944-FF6D-4D6C-A98E-0901F771B584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="elasFU_CES" sheetId="5" r:id="rId1"/>
@@ -21,12 +21,22 @@
     <sheet name="elasKL-E" sheetId="11" r:id="rId6"/>
     <sheet name="prodKL-E" sheetId="12" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="100">
   <si>
     <t>elasIU_DM</t>
   </si>
@@ -64,87 +74,18 @@
     <t>GOS</t>
   </si>
   <si>
-    <t>pFBTO</t>
-  </si>
-  <si>
-    <t>pTXWO</t>
-  </si>
-  <si>
-    <t>pCOKE</t>
-  </si>
-  <si>
-    <t>pREFN</t>
-  </si>
-  <si>
-    <t>pCHEM</t>
-  </si>
-  <si>
-    <t>pRUBP</t>
-  </si>
-  <si>
-    <t>pNMMP</t>
-  </si>
-  <si>
-    <t>pMETP</t>
-  </si>
-  <si>
     <t>pELEC</t>
   </si>
   <si>
-    <t>pMACH</t>
-  </si>
-  <si>
     <t>pTRDI</t>
   </si>
   <si>
-    <t>pHWAT</t>
-  </si>
-  <si>
-    <t>pWATR</t>
-  </si>
-  <si>
-    <t>iFBTO</t>
-  </si>
-  <si>
-    <t>iTXWO</t>
-  </si>
-  <si>
-    <t>iCOKE</t>
-  </si>
-  <si>
-    <t>iREFN</t>
-  </si>
-  <si>
-    <t>iCHEM</t>
-  </si>
-  <si>
-    <t>iRUBP</t>
-  </si>
-  <si>
-    <t>iNMMP</t>
-  </si>
-  <si>
-    <t>iMETP</t>
-  </si>
-  <si>
-    <t>iELEC</t>
-  </si>
-  <si>
-    <t>iMACH</t>
-  </si>
-  <si>
     <t>iELCG</t>
   </si>
   <si>
     <t>iTRDI</t>
   </si>
   <si>
-    <t>iHWAT</t>
-  </si>
-  <si>
-    <t>iWATR</t>
-  </si>
-  <si>
     <t>elasKLE</t>
   </si>
   <si>
@@ -211,34 +152,190 @@
     <t>iELCS</t>
   </si>
   <si>
-    <t>iELCP</t>
-  </si>
-  <si>
-    <t>iELCM</t>
-  </si>
-  <si>
     <t>iELCE</t>
   </si>
   <si>
-    <t>pFOOD</t>
-  </si>
-  <si>
-    <t>pMINE</t>
-  </si>
-  <si>
-    <t>pELCC</t>
-  </si>
-  <si>
     <t>pSERV</t>
   </si>
   <si>
-    <t>iMINE</t>
-  </si>
-  <si>
     <t>iSERV</t>
   </si>
   <si>
-    <t>iFOOD</t>
+    <t>pAGRI</t>
+  </si>
+  <si>
+    <t>pINDU</t>
+  </si>
+  <si>
+    <t>pALUM</t>
+  </si>
+  <si>
+    <t>pTRAN</t>
+  </si>
+  <si>
+    <t>pHTWT</t>
+  </si>
+  <si>
+    <t>pOIL</t>
+  </si>
+  <si>
+    <t>pGSL</t>
+  </si>
+  <si>
+    <t>pDSL</t>
+  </si>
+  <si>
+    <t>pHDI</t>
+  </si>
+  <si>
+    <t>pNG</t>
+  </si>
+  <si>
+    <t>pCOA</t>
+  </si>
+  <si>
+    <t>pBIO</t>
+  </si>
+  <si>
+    <t>pFUL</t>
+  </si>
+  <si>
+    <t>iAGRI</t>
+  </si>
+  <si>
+    <t>iCOAL</t>
+  </si>
+  <si>
+    <t>iCOIL</t>
+  </si>
+  <si>
+    <t>iINDU</t>
+  </si>
+  <si>
+    <t>iALUM</t>
+  </si>
+  <si>
+    <t>iNGAS</t>
+  </si>
+  <si>
+    <t>iTRAN</t>
+  </si>
+  <si>
+    <t>KL</t>
+  </si>
+  <si>
+    <t>KLE</t>
+  </si>
+  <si>
+    <t>KLEM</t>
+  </si>
+  <si>
+    <t>AAGR</t>
+  </si>
+  <si>
+    <t>COAL</t>
+  </si>
+  <si>
+    <t>COIL</t>
+  </si>
+  <si>
+    <t>IMIN</t>
+  </si>
+  <si>
+    <t>IRES</t>
+  </si>
+  <si>
+    <t>IALA</t>
+  </si>
+  <si>
+    <t>POWF</t>
+  </si>
+  <si>
+    <t>POWR</t>
+  </si>
+  <si>
+    <t>POWT</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>LTH</t>
+  </si>
+  <si>
+    <t>COTH</t>
+  </si>
+  <si>
+    <t>CCON</t>
+  </si>
+  <si>
+    <t>CWSR</t>
+  </si>
+  <si>
+    <t>COFF</t>
+  </si>
+  <si>
+    <t>C_TRAI</t>
+  </si>
+  <si>
+    <t>C_TLND</t>
+  </si>
+  <si>
+    <t>C_TPIP</t>
+  </si>
+  <si>
+    <t>C_TWAS</t>
+  </si>
+  <si>
+    <t>C_TWAI</t>
+  </si>
+  <si>
+    <t>C_TAIR</t>
+  </si>
+  <si>
+    <t>CHEA</t>
+  </si>
+  <si>
+    <t>Waste</t>
+  </si>
+  <si>
+    <t>BIO</t>
+  </si>
+  <si>
+    <t>i-AGR</t>
+  </si>
+  <si>
+    <t>i-COAL</t>
+  </si>
+  <si>
+    <t>i-COIL</t>
+  </si>
+  <si>
+    <t>i-IND</t>
+  </si>
+  <si>
+    <t>i-ALA</t>
+  </si>
+  <si>
+    <t>i-POWF</t>
+  </si>
+  <si>
+    <t>i-POWR</t>
+  </si>
+  <si>
+    <t>i-POWT</t>
+  </si>
+  <si>
+    <t>i-NG</t>
+  </si>
+  <si>
+    <t>i-SERV</t>
+  </si>
+  <si>
+    <t>i-TRA</t>
+  </si>
+  <si>
+    <t>---</t>
   </si>
 </sst>
 </file>
@@ -639,7 +736,7 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1"/>
@@ -686,29 +783,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:22">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>0.32</v>
@@ -717,23 +814,26 @@
         <v>-1.54</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:22">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B3">
-        <v>0.32</v>
+        <v>1.29</v>
       </c>
       <c r="C3">
         <v>-1.54</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>21</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <v>0.32</v>
@@ -742,51 +842,63 @@
         <v>-1.54</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>25</v>
+      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B5">
-        <v>0.82</v>
+        <v>1.29</v>
       </c>
       <c r="C5">
         <v>-1.54</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>22</v>
+      </c>
+      <c r="T5" s="1"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B6">
-        <v>0.97</v>
+        <v>1.23</v>
       </c>
       <c r="C6">
         <v>-1.54</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="T6" s="1"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>0.97</v>
+        <v>1.04</v>
       </c>
       <c r="C7">
         <v>-1.54</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>23</v>
+      </c>
+      <c r="T7" s="1"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>1.29</v>
@@ -794,65 +906,83 @@
       <c r="C8">
         <v>-1.54</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="T8" s="1"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B9">
-        <v>1.29</v>
+        <v>1.04</v>
       </c>
       <c r="C9">
         <v>-1.54</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="T9" s="1"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B10">
-        <v>1.29</v>
+        <v>0.97</v>
       </c>
       <c r="C10">
         <v>-1.54</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="T10" s="1"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11">
-        <v>1.29</v>
+        <v>47</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.97</v>
       </c>
       <c r="C11">
         <v>-1.54</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="T11" s="1"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12">
-        <v>1.04</v>
+        <v>48</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.97</v>
       </c>
       <c r="C12">
         <v>-1.54</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="T12" s="1"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13">
-        <v>1.04</v>
+        <v>49</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.97</v>
       </c>
       <c r="C13">
         <v>-1.54</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="T13" s="1"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B14" s="4">
         <v>0.97</v>
@@ -860,86 +990,101 @@
       <c r="C14" s="4">
         <v>-1.54</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="T14" s="1"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15">
+        <v>51</v>
+      </c>
+      <c r="B15" s="4">
         <v>0.97</v>
       </c>
       <c r="C15">
         <v>-1.54</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="T15" s="1"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16">
+        <v>52</v>
+      </c>
+      <c r="B16" s="4">
         <v>0.97</v>
       </c>
       <c r="C16">
         <v>-1.54</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="T16" s="1"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17">
-        <v>1.29</v>
+        <v>53</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.97</v>
       </c>
       <c r="C17">
         <v>-1.54</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="T17" s="1"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="T18" s="1"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" s="1"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:22">
       <c r="A20" s="1"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:22">
       <c r="A21" s="1"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:22">
       <c r="A22" s="1"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:22">
       <c r="A23" s="1"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:22">
       <c r="A24" s="1"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:22">
       <c r="A25" s="1"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="27" spans="1:3" s="4" customFormat="1"/>
-    <row r="28" spans="1:3" s="4" customFormat="1"/>
-    <row r="29" spans="1:3" s="4" customFormat="1"/>
-    <row r="30" spans="1:3" s="4" customFormat="1"/>
-    <row r="31" spans="1:3" s="4" customFormat="1"/>
-    <row r="32" spans="1:3" s="4" customFormat="1"/>
+    <row r="27" spans="1:22" s="4" customFormat="1"/>
+    <row r="28" spans="1:22" s="4" customFormat="1"/>
+    <row r="29" spans="1:22" s="4" customFormat="1"/>
+    <row r="30" spans="1:22" s="4" customFormat="1"/>
+    <row r="31" spans="1:22" s="4" customFormat="1"/>
+    <row r="32" spans="1:22" s="4" customFormat="1"/>
     <row r="33" spans="1:1" s="4" customFormat="1"/>
     <row r="34" spans="1:1" s="4" customFormat="1"/>
     <row r="35" spans="1:1" s="4" customFormat="1"/>
@@ -970,15 +1115,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:13">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -992,30 +1137,30 @@
         <v>8</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2">
+        <v>41</v>
+      </c>
+      <c r="B2" s="4">
         <v>3</v>
       </c>
       <c r="C2" s="4">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>5</v>
       </c>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
@@ -1023,19 +1168,19 @@
       <c r="C3" s="4">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>5</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>5</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B4" s="4">
         <v>3</v>
@@ -1043,19 +1188,19 @@
       <c r="C4" s="4">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>5</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B5" s="4">
         <v>3</v>
@@ -1063,19 +1208,19 @@
       <c r="C5" s="4">
         <v>3</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>5</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>5</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B6" s="4">
         <v>3</v>
@@ -1083,67 +1228,67 @@
       <c r="C6" s="4">
         <v>3</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4">
-        <v>3</v>
+        <v>0.3</v>
       </c>
       <c r="C7" s="4">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8" s="4">
-        <v>3</v>
+        <v>0.3</v>
       </c>
       <c r="C8" s="4">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>0.3</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B9" s="4">
-        <v>3</v>
+        <v>0.3</v>
       </c>
       <c r="C9" s="4">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>0.3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B10" s="4">
         <v>3</v>
@@ -1151,16 +1296,16 @@
       <c r="C10" s="4">
         <v>3</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>5</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B11" s="4">
         <v>3</v>
@@ -1168,16 +1313,21 @@
       <c r="C11" s="4">
         <v>3</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>5</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="1"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B12" s="4">
         <v>3</v>
@@ -1185,16 +1335,21 @@
       <c r="C12" s="4">
         <v>3</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>5</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" s="1"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B13" s="4">
         <v>3</v>
@@ -1202,121 +1357,193 @@
       <c r="C13" s="4">
         <v>3</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>5</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" s="1"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B14" s="4">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="C14" s="4">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="D14" s="4">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="E14" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>5</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B15" s="4">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="C15" s="4">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="D15" s="4">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="E15" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>5</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B16" s="4">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="C16" s="4">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="D16" s="4">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="E16" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>5</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="B17" s="4">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="C17" s="4">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="D17" s="4">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="E17" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="4">
-        <v>3</v>
-      </c>
-      <c r="C18" s="4">
-        <v>3</v>
-      </c>
-      <c r="D18">
         <v>5</v>
       </c>
-      <c r="E18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="I17" s="1"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="1"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="I19" s="1"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="I20" s="1"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="I21" s="1"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="I22" s="1"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="I23" s="1"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="I24" s="1"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="I25" s="1"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="1"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" s="4" customFormat="1">
+      <c r="I26" s="1"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+    </row>
+    <row r="27" spans="1:13" s="4" customFormat="1">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:5" s="4" customFormat="1">
+    <row r="28" spans="1:13" s="4" customFormat="1">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:5" s="4" customFormat="1">
+    <row r="29" spans="1:13" s="4" customFormat="1">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:5" s="4" customFormat="1">
+    <row r="30" spans="1:13" s="4" customFormat="1">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:5" s="4" customFormat="1">
+    <row r="31" spans="1:13" s="4" customFormat="1">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:5" s="4" customFormat="1">
+    <row r="32" spans="1:13" s="4" customFormat="1">
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:3" s="4" customFormat="1">
@@ -1371,11 +1598,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B29" sqref="A2:B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
@@ -1384,227 +1611,190 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2">
-        <v>0.95</v>
+        <v>54</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.29535</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3">
-        <v>0.95</v>
+        <v>55</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1.2801</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4">
-        <v>0.95</v>
+        <v>56</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.31059999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5">
-        <v>0.95</v>
+        <v>57</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.5952599999999999</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6">
-        <v>0.95</v>
+        <v>58</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.28660000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7">
-        <v>0.95</v>
+        <v>15</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.30209999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8">
-        <v>0.95</v>
+        <v>59</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.30209999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9">
-        <v>0.95</v>
+        <v>40</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.32832499999999998</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10">
-        <v>0.95</v>
+        <v>60</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.57545000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11">
-        <v>0.95</v>
+        <v>30</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.30209999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12">
-        <v>0.95</v>
+        <v>14</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.30209999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13">
-        <v>0.95</v>
+        <v>32</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.30209999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14">
-        <v>0.95</v>
+        <v>33</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.30209999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B15" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B16" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B17" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B18" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B19" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B20" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="4">
-        <v>0.95</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="4">
-        <v>0.95</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="4">
-        <v>0.95</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="4">
-        <v>0.95</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25">
-        <v>0.95</v>
-      </c>
+      <c r="A25" s="1"/>
     </row>
     <row r="26" spans="1:2" s="4" customFormat="1">
-      <c r="A26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26">
-        <v>0.95</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="B26"/>
     </row>
     <row r="27" spans="1:2" s="4" customFormat="1">
-      <c r="A27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27">
-        <v>0.95</v>
-      </c>
+      <c r="A27" s="1"/>
+      <c r="B27"/>
     </row>
     <row r="28" spans="1:2" s="4" customFormat="1">
-      <c r="A28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28">
-        <v>0.95</v>
-      </c>
+      <c r="A28" s="1"/>
+      <c r="B28"/>
     </row>
     <row r="29" spans="1:2" s="4" customFormat="1">
-      <c r="A29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29">
-        <v>0.95</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="B29"/>
     </row>
     <row r="30" spans="1:2" s="4" customFormat="1"/>
     <row r="31" spans="1:2" s="4" customFormat="1"/>
@@ -1639,11 +1829,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="A2:C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" t="s">
@@ -1655,7 +1845,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1666,7 +1856,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -1677,7 +1867,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -1688,7 +1878,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
@@ -1699,7 +1889,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
@@ -1710,7 +1900,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
@@ -1721,7 +1911,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -1732,7 +1922,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -1743,7 +1933,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
@@ -1754,7 +1944,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="4">
         <v>1</v>
@@ -1765,7 +1955,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
@@ -1776,7 +1966,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="4">
         <v>1</v>
@@ -1787,7 +1977,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
@@ -1798,7 +1988,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
@@ -1809,7 +1999,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
@@ -1820,7 +2010,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
@@ -1831,7 +2021,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
@@ -1842,7 +2032,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
@@ -1853,7 +2043,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
@@ -1863,103 +2053,41 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4">
-        <v>1</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4">
-        <v>1</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="4">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4">
-        <v>1</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="4">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4">
-        <v>1</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:3" s="4" customFormat="1">
-      <c r="A26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="4">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4">
-        <v>1</v>
-      </c>
+      <c r="A26" s="1"/>
     </row>
     <row r="27" spans="1:3" s="4" customFormat="1">
-      <c r="A27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4">
-        <v>1</v>
-      </c>
+      <c r="A27" s="1"/>
     </row>
     <row r="28" spans="1:3" s="4" customFormat="1">
-      <c r="A28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="4">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4">
-        <v>1</v>
-      </c>
+      <c r="A28" s="1"/>
     </row>
     <row r="29" spans="1:3" s="4" customFormat="1">
-      <c r="A29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="4">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4">
-        <v>1</v>
-      </c>
+      <c r="A29" s="1"/>
     </row>
     <row r="30" spans="1:3" s="4" customFormat="1">
       <c r="A30" s="1"/>
@@ -2019,426 +2147,1214 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:23">
       <c r="B1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>17</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B2" s="4">
-        <v>0.4</v>
+        <v>2.84815</v>
       </c>
       <c r="C2" s="4">
-        <v>0.95</v>
+        <v>0.29535</v>
       </c>
       <c r="D2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="J2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0.34129999999999999</v>
+      </c>
+      <c r="M2" s="4">
+        <v>5.2298</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0.78149999999999997</v>
+      </c>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="S2" s="4">
+        <f>AVERAGEIF($J$2:$J$25,$R2,L$2:L$25)</f>
+        <v>0.29535</v>
+      </c>
+      <c r="T2" s="4">
+        <f t="shared" ref="T2:U12" si="0">AVERAGEIF($J$2:$J$25,$R2,M$2:M$25)</f>
+        <v>2.84815</v>
+      </c>
+      <c r="U2" s="4">
+        <f t="shared" si="0"/>
+        <v>0.96675</v>
+      </c>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4">
-        <v>0.4</v>
+        <v>0.53959999999999997</v>
       </c>
       <c r="C3" s="4">
-        <v>0.95</v>
+        <v>1.2801</v>
       </c>
       <c r="D3" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="J3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1.2801</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0.53959999999999997</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0.26590000000000003</v>
+      </c>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="S3" s="4">
+        <f t="shared" ref="S3:S12" si="1">AVERAGEIF($J$2:$J$25,$R3,L$2:L$25)</f>
+        <v>1.2801</v>
+      </c>
+      <c r="T3" s="4">
+        <f t="shared" si="0"/>
+        <v>0.53959999999999997</v>
+      </c>
+      <c r="U3" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26590000000000003</v>
+      </c>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4">
-        <v>0.4</v>
+        <v>7.8575999999999997</v>
       </c>
       <c r="C4" s="4">
-        <v>0.95</v>
+        <v>0.31059999999999999</v>
       </c>
       <c r="D4" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="J4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.31059999999999999</v>
+      </c>
+      <c r="M4" s="4">
+        <v>7.8575999999999997</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0.3075</v>
+      </c>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="S4" s="4">
+        <f t="shared" si="1"/>
+        <v>0.31059999999999999</v>
+      </c>
+      <c r="T4" s="4">
+        <f t="shared" si="0"/>
+        <v>7.8575999999999997</v>
+      </c>
+      <c r="U4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.3075</v>
+      </c>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B5" s="4">
-        <v>0.4</v>
+        <v>0.24174999999999999</v>
       </c>
       <c r="C5" s="4">
-        <v>0.95</v>
+        <v>0.5952599999999999</v>
       </c>
       <c r="D5" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="J5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1.2801</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0.53959999999999997</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0.26590000000000003</v>
+      </c>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="S5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.5952599999999999</v>
+      </c>
+      <c r="T5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.24174999999999999</v>
+      </c>
+      <c r="U5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.78743999999999992</v>
+      </c>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="B6" s="4">
-        <v>0.4</v>
+        <v>0.86909999999999998</v>
       </c>
       <c r="C6" s="4">
-        <v>0.95</v>
+        <v>0.28660000000000002</v>
       </c>
       <c r="D6" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="J6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0.26250000000000001</v>
+      </c>
+      <c r="M6" s="4">
+        <v>9.5799999999999996E-2</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0.62090000000000001</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="S6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.28660000000000002</v>
+      </c>
+      <c r="T6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.86909999999999998</v>
+      </c>
+      <c r="U6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.64290000000000003</v>
+      </c>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
-        <v>0.4</v>
+        <v>0.2757</v>
       </c>
       <c r="C7" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
       <c r="D7" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="J7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.28660000000000002</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0.86909999999999998</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0.64290000000000003</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="S7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="T7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2757</v>
+      </c>
+      <c r="U7" s="4">
+        <f t="shared" si="0"/>
+        <v>1.196</v>
+      </c>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B8" s="4">
-        <v>0.4</v>
+        <v>0.2757</v>
       </c>
       <c r="C8" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
       <c r="D8" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="J8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0.2757</v>
+      </c>
+      <c r="N8" s="4">
+        <v>1.196</v>
+      </c>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="S8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="T8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2757</v>
+      </c>
+      <c r="U8" s="4">
+        <f t="shared" si="0"/>
+        <v>1.196</v>
+      </c>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B9" s="4">
-        <v>0.4</v>
+        <v>0.74172499999999997</v>
       </c>
       <c r="C9" s="4">
-        <v>0.95</v>
+        <v>0.32832499999999998</v>
       </c>
       <c r="D9" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="J9" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0.2757</v>
+      </c>
+      <c r="N9" s="4">
+        <v>1.196</v>
+      </c>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="S9" s="4">
+        <f t="shared" si="1"/>
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="T9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2757</v>
+      </c>
+      <c r="U9" s="4">
+        <f t="shared" si="0"/>
+        <v>1.196</v>
+      </c>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B10" s="4">
-        <v>0.4</v>
+        <v>0.72006666666666652</v>
       </c>
       <c r="C10" s="4">
-        <v>0.95</v>
+        <v>0.57545000000000002</v>
       </c>
       <c r="D10" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="J10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0.2757</v>
+      </c>
+      <c r="N10" s="4">
+        <v>1.196</v>
+      </c>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="S10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="T10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2757</v>
+      </c>
+      <c r="U10" s="4">
+        <f t="shared" si="0"/>
+        <v>1.196</v>
+      </c>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="4">
-        <v>0.4</v>
+        <v>0.2757</v>
       </c>
       <c r="C11" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
       <c r="D11" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="J11" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0.2757</v>
+      </c>
+      <c r="N11" s="4">
+        <v>1.196</v>
+      </c>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="S11" s="4">
+        <f t="shared" si="1"/>
+        <v>0.32832499999999998</v>
+      </c>
+      <c r="T11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.74172499999999997</v>
+      </c>
+      <c r="U11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.87357499999999999</v>
+      </c>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B12" s="4">
-        <v>0.4</v>
+        <v>0.2757</v>
       </c>
       <c r="C12" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
       <c r="D12" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="J12" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0.2757</v>
+      </c>
+      <c r="N12" s="4">
+        <v>1.196</v>
+      </c>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="S12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.57545000000000002</v>
+      </c>
+      <c r="T12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.72006666666666652</v>
+      </c>
+      <c r="U12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.88693333333333335</v>
+      </c>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="4">
-        <v>0.4</v>
+        <v>0.2757</v>
       </c>
       <c r="C13" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
       <c r="D13" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="J13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0.29859999999999998</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1.1994</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0.83730000000000004</v>
+      </c>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S13" s="4">
+        <f>S$7</f>
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="T13" s="4">
+        <f t="shared" ref="T13:U14" si="2">T$7</f>
+        <v>0.2757</v>
+      </c>
+      <c r="U13" s="4">
+        <f t="shared" si="2"/>
+        <v>1.196</v>
+      </c>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B14" s="4">
-        <v>0.4</v>
+        <v>0.2757</v>
       </c>
       <c r="C14" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
       <c r="D14" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="J14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0.30669999999999997</v>
+      </c>
+      <c r="M14" s="4">
+        <v>5.5899999999999998E-2</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0.70630000000000004</v>
+      </c>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S14" s="4">
+        <f>S$7</f>
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="T14" s="4">
+        <f t="shared" si="2"/>
+        <v>0.2757</v>
+      </c>
+      <c r="U14" s="4">
+        <f t="shared" si="2"/>
+        <v>1.196</v>
+      </c>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B15" s="4">
-        <v>0.4</v>
+        <v>0.2757</v>
       </c>
       <c r="C15" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
       <c r="D15" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="J15" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0.1973</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0.20519999999999999</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0.68089999999999995</v>
+      </c>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S15" s="4">
+        <f t="shared" ref="S15:U22" si="3">S$7</f>
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="T15" s="4">
+        <f t="shared" si="3"/>
+        <v>0.2757</v>
+      </c>
+      <c r="U15" s="4">
+        <f t="shared" si="3"/>
+        <v>1.196</v>
+      </c>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B16" s="4">
-        <v>0.4</v>
+        <v>0.2757</v>
       </c>
       <c r="C16" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
       <c r="D16" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="J16" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="M16" s="4">
+        <v>1.0958000000000001</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0.82410000000000005</v>
+      </c>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S16" s="4">
+        <f t="shared" si="3"/>
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="T16" s="4">
+        <f t="shared" si="3"/>
+        <v>0.2757</v>
+      </c>
+      <c r="U16" s="4">
+        <f t="shared" si="3"/>
+        <v>1.196</v>
+      </c>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B17" s="4">
-        <v>0.4</v>
+        <v>0.2757</v>
       </c>
       <c r="C17" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
       <c r="D17" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="J17" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0.86709999999999998</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0.22289999999999999</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0.91890000000000005</v>
+      </c>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S17" s="4">
+        <f t="shared" si="3"/>
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="T17" s="4">
+        <f t="shared" si="3"/>
+        <v>0.2757</v>
+      </c>
+      <c r="U17" s="4">
+        <f t="shared" si="3"/>
+        <v>1.196</v>
+      </c>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B18" s="4">
-        <v>0.4</v>
+        <v>0.2757</v>
       </c>
       <c r="C18" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
       <c r="D18" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="J18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0.86709999999999998</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0.22289999999999999</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0.91890000000000005</v>
+      </c>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S18" s="4">
+        <f t="shared" si="3"/>
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="T18" s="4">
+        <f t="shared" si="3"/>
+        <v>0.2757</v>
+      </c>
+      <c r="U18" s="4">
+        <f t="shared" si="3"/>
+        <v>1.196</v>
+      </c>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" s="1" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B19" s="4">
-        <v>0.4</v>
+        <v>0.2757</v>
       </c>
       <c r="C19" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
       <c r="D19" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="J19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0.29859999999999998</v>
+      </c>
+      <c r="M19" s="4">
+        <v>1.1994</v>
+      </c>
+      <c r="N19" s="4">
+        <v>0.83730000000000004</v>
+      </c>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S19" s="4">
+        <f t="shared" si="3"/>
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="T19" s="4">
+        <f t="shared" si="3"/>
+        <v>0.2757</v>
+      </c>
+      <c r="U19" s="4">
+        <f t="shared" si="3"/>
+        <v>1.196</v>
+      </c>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B20" s="4">
-        <v>0.4</v>
+        <v>0.2757</v>
       </c>
       <c r="C20" s="4">
-        <v>0.95</v>
+        <v>0.30209999999999998</v>
       </c>
       <c r="D20" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C21" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="D22" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C23" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="D23" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C24" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C25" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="D25" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1" t="s">
+      <c r="J20" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0.29859999999999998</v>
+      </c>
+      <c r="M20" s="4">
+        <v>1.1994</v>
+      </c>
+      <c r="N20" s="4">
+        <v>0.83730000000000004</v>
+      </c>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S20" s="4">
+        <f t="shared" si="3"/>
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="T20" s="4">
+        <f t="shared" si="3"/>
+        <v>0.2757</v>
+      </c>
+      <c r="U20" s="4">
+        <f t="shared" si="3"/>
+        <v>1.196</v>
+      </c>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+    </row>
+    <row r="21" spans="1:23">
+      <c r="A21" s="1"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="J21" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0.29859999999999998</v>
+      </c>
+      <c r="M21" s="4">
+        <v>1.1994</v>
+      </c>
+      <c r="N21" s="4">
+        <v>0.83730000000000004</v>
+      </c>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S21" s="4">
+        <f t="shared" si="3"/>
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="T21" s="4">
+        <f t="shared" si="3"/>
+        <v>0.2757</v>
+      </c>
+      <c r="U21" s="4">
+        <f t="shared" si="3"/>
+        <v>1.196</v>
+      </c>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22" s="1"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="J22" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0.82269999999999999</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0.27639999999999998</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0.97189999999999999</v>
+      </c>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C26" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="D26" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="4" customFormat="1">
-      <c r="A27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C27" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="4" customFormat="1">
-      <c r="A28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C28" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="D28" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="4" customFormat="1">
-      <c r="A29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C29" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="4" customFormat="1">
+      <c r="R22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S22" s="4">
+        <f t="shared" si="3"/>
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="T22" s="4">
+        <f t="shared" si="3"/>
+        <v>0.2757</v>
+      </c>
+      <c r="U22" s="4">
+        <f t="shared" si="3"/>
+        <v>1.196</v>
+      </c>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23" s="1"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="J23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0.82489999999999997</v>
+      </c>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4">
+        <v>1.1480999999999999</v>
+      </c>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+    </row>
+    <row r="24" spans="1:23">
+      <c r="A24" s="1"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="J24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L24" s="4">
+        <v>0.24940000000000001</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0.46650000000000003</v>
+      </c>
+      <c r="N24" s="4">
+        <v>1.1519999999999999</v>
+      </c>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="4"/>
+      <c r="W24" s="4"/>
+    </row>
+    <row r="25" spans="1:23">
+      <c r="A25" s="1"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="J25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L25" s="4">
+        <v>0.24940000000000001</v>
+      </c>
+      <c r="M25" s="4">
+        <v>0.46650000000000003</v>
+      </c>
+      <c r="N25" s="4">
+        <v>1.1519999999999999</v>
+      </c>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+    </row>
+    <row r="26" spans="1:23">
+      <c r="A26" s="1"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:23" s="4" customFormat="1">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:23" s="4" customFormat="1">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:23" s="4" customFormat="1">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:23" s="4" customFormat="1">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:4" s="4" customFormat="1">
+    <row r="31" spans="1:23" s="4" customFormat="1">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:4" s="4" customFormat="1">
+    <row r="32" spans="1:23" s="4" customFormat="1">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
     </row>
@@ -2505,15 +3421,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:U25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:21">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -2521,12 +3437,19 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>18</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -2537,10 +3460,18 @@
       <c r="D2" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -2551,10 +3482,19 @@
       <c r="D3" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -2565,10 +3505,19 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
@@ -2579,10 +3528,19 @@
       <c r="D5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
@@ -2593,10 +3551,19 @@
       <c r="D6" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
@@ -2607,10 +3574,19 @@
       <c r="D7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -2621,123 +3597,188 @@
       <c r="D8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="P13" s="4"/>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="P14" s="4"/>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="P15" s="4"/>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="4">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="P16" s="4"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="4">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="4">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="4">
-        <v>1</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="B17" s="4">
         <v>1</v>
       </c>
@@ -2747,10 +3788,15 @@
       <c r="D17" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="P17" s="4"/>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
@@ -2761,10 +3807,15 @@
       <c r="D18" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="P18" s="4"/>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="1" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
@@ -2775,10 +3826,15 @@
       <c r="D19" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="P19" s="4"/>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
@@ -2789,140 +3845,89 @@
       <c r="D20" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4">
-        <v>1</v>
-      </c>
-      <c r="D22" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4">
-        <v>1</v>
-      </c>
-      <c r="D23" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="4">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4">
-        <v>1</v>
-      </c>
-      <c r="D24" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="4">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4">
-        <v>1</v>
-      </c>
-      <c r="D25" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="4">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4">
-        <v>1</v>
-      </c>
-      <c r="D26" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="4" customFormat="1">
-      <c r="A27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4">
-        <v>1</v>
-      </c>
-      <c r="D27" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="4" customFormat="1">
-      <c r="A28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="4">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4">
-        <v>1</v>
-      </c>
-      <c r="D28" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="4" customFormat="1">
-      <c r="A29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="4">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4">
-        <v>1</v>
-      </c>
-      <c r="D29" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="4" customFormat="1">
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="P20" s="4"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="1"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="P21" s="4"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="1"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="P22" s="4"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="1"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="P23" s="4"/>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="1"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="P24" s="4"/>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="1"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="P25" s="4"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="1"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:16" s="4" customFormat="1">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" s="4" customFormat="1">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:16" s="4" customFormat="1">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" s="4" customFormat="1">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:4" s="4" customFormat="1">
+    <row r="31" spans="1:16" s="4" customFormat="1">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:4" s="4" customFormat="1">
+    <row r="32" spans="1:16" s="4" customFormat="1">
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" s="4" customFormat="1">

</xml_diff>

<commit_message>
Add hydrogen (H2) product to database
 And run some simulation

01_BAU_new: uses a new way to match GDP: increate KS and increase prodK and prodL.
</commit_message>
<xml_diff>
--- a/project_open_entrance/00_base_model_setup/data/Eldata.xlsx
+++ b/project_open_entrance/00_base_model_setup/data/Eldata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boonmanhj\Documents\Gitlab\TNO-Eco-Mod-CI\project_open_entrance\00_base_model_setup\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boonmanhj\Documents\Gitlab\tno-eco-mod-ci\project_open_entrance\00_base_model_setup\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D6F944-FF6D-4D6C-A98E-0901F771B584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891F6E13-DC48-4485-9419-788C61E8F991}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="elasFU_CES" sheetId="5" r:id="rId1"/>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="101">
   <si>
     <t>elasIU_DM</t>
   </si>
@@ -336,6 +334,9 @@
   </si>
   <si>
     <t>---</t>
+  </si>
+  <si>
+    <t>iH2</t>
   </si>
 </sst>
 </file>
@@ -732,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1599,7 +1600,7 @@
   <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1762,8 +1763,12 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0.30209999999999998</v>
+      </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1"/>
@@ -1830,7 +1835,7 @@
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2053,9 +2058,15 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="A21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1"/>
@@ -2149,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3158,10 +3169,18 @@
       <c r="W20" s="4"/>
     </row>
     <row r="21" spans="1:23">
-      <c r="A21" s="1"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="A21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0.2757</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.5</v>
+      </c>
       <c r="J21" s="4" t="s">
         <v>98</v>
       </c>
@@ -3424,7 +3443,7 @@
   <dimension ref="A1:U46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:U25"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3852,10 +3871,18 @@
       <c r="P20" s="4"/>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="1"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="A21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>

</xml_diff>